<commit_message>
vijaya s data driven scrits
</commit_message>
<xml_diff>
--- a/TestData/ContactUsFormData.xlsx
+++ b/TestData/ContactUsFormData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijayalakshmi B\git\Datadrivenframework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1B5393-29C6-4542-BEE7-9F771D32E8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DBAD20-9B54-4BB4-8C88-BE4BADD8CE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="2676" windowWidth="17280" windowHeight="8964" xr2:uid="{9A53E665-38C9-4C5B-B7C0-1BBF62DE05D8}"/>
+    <workbookView xWindow="4092" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{9A53E665-38C9-4C5B-B7C0-1BBF62DE05D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>abc@gmail.com</t>
   </si>
@@ -33,9 +33,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>XYZ</t>
   </si>
   <si>
@@ -63,15 +60,6 @@
     <t>Business Banking</t>
   </si>
   <si>
-    <t>lmn</t>
-  </si>
-  <si>
-    <t>LMN</t>
-  </si>
-  <si>
-    <t>pqr</t>
-  </si>
-  <si>
     <t>PQR</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
     <t>pqr@gmail.com</t>
   </si>
   <si>
-    <t>sample text</t>
-  </si>
-  <si>
     <t>query text</t>
   </si>
   <si>
@@ -97,13 +82,25 @@
   </si>
   <si>
     <t>2267890</t>
+  </si>
+  <si>
+    <t>abcdefghipqrstuvwxyz</t>
+  </si>
+  <si>
+    <t>lmnopqrstuvwxy</t>
+  </si>
+  <si>
+    <t>abcdefpqrstuvwxyz</t>
+  </si>
+  <si>
+    <t>987654322</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +112,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -460,19 +463,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277FD8C2-4454-4496-A554-8EAB4A5CFB32}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -480,89 +485,111 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" xr:uid="{BFF96ED1-A39D-46A4-BD7E-353382EC4779}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{50076042-3DB1-4C8C-A0AB-A9AD7791C1F7}"/>
     <hyperlink ref="D3" r:id="rId3" xr:uid="{AD22F825-5592-4AF9-9738-E6B62A22A730}"/>
     <hyperlink ref="D4" r:id="rId4" xr:uid="{437405FF-2BBC-4FE6-BBFE-FD2D69B01DC1}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{2B7C55EC-1DE5-4DD3-AACC-8A7C3255E6FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>